<commit_message>
gathered all the params from old db
</commit_message>
<xml_diff>
--- a/pics.xlsx
+++ b/pics.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\elemental\vindenatt.github.io\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E882260C-F5AE-45BF-8136-0B6DC7EA86EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11952" windowHeight="5220"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -101,31 +102,31 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="ＭＳ Ｐゴシック"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="Calibri"/>
+      <name val="ＭＳ Ｐゴシック"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <family val="2"/>
+      <sz val="6"/>
+      <name val="ＭＳ Ｐゴシック"/>
+      <family val="3"/>
+      <charset val="128"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -135,11 +136,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
   </fills>
@@ -152,23 +148,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="0" xfId="2" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="3">
-    <cellStyle name="Good" xfId="1" builtinId="26"/>
-    <cellStyle name="Neutral" xfId="2" builtinId="28"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  <cellStyles count="2">
+    <cellStyle name="標準" xfId="0" builtinId="0"/>
+    <cellStyle name="良い" xfId="1" builtinId="26"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -445,19 +437,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="A2" sqref="A2:C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="14.109375" customWidth="1"/>
+    <col min="1" max="1" width="14.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A1" s="2" t="s">
         <v>18</v>
       </c>
@@ -468,111 +460,112 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="4" t="s">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A2" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="4" t="s">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A3" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A4" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A5" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B6" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B7" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B8" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B9" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B10" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B11" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B12" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B13" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B14" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B15" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B16" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B17" s="1" t="s">
         <v>16</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
new features in master
</commit_message>
<xml_diff>
--- a/pics.xlsx
+++ b/pics.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\elemental\vindenatt.github.io\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\vindenatt.github.io-1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E882260C-F5AE-45BF-8136-0B6DC7EA86EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="26">
   <si>
     <t>01</t>
   </si>
@@ -97,30 +96,36 @@
   </si>
   <si>
     <t>450-499</t>
+  </si>
+  <si>
+    <t>500-599</t>
+  </si>
+  <si>
+    <t>600-699</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="ＭＳ Ｐゴシック"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="ＭＳ Ｐゴシック"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="6"/>
-      <name val="ＭＳ Ｐゴシック"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -159,8 +164,8 @@
     <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="標準" xfId="0" builtinId="0"/>
-    <cellStyle name="良い" xfId="1" builtinId="26"/>
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -437,19 +442,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:C5"/>
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="14.125" customWidth="1"/>
+    <col min="1" max="1" width="14.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:3">
       <c r="A1" s="2" t="s">
         <v>18</v>
       </c>
@@ -460,7 +465,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:3">
       <c r="A2" s="2" t="s">
         <v>20</v>
       </c>
@@ -471,7 +476,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:3">
       <c r="A3" s="2" t="s">
         <v>21</v>
       </c>
@@ -482,7 +487,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:3">
       <c r="A4" s="2" t="s">
         <v>22</v>
       </c>
@@ -493,7 +498,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:3">
       <c r="A5" s="2" t="s">
         <v>23</v>
       </c>
@@ -504,62 +509,74 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:3">
+      <c r="A6" t="s">
+        <v>24</v>
+      </c>
       <c r="B6" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="C6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" t="s">
+        <v>25</v>
+      </c>
       <c r="B7" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="C7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
       <c r="B8" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:3">
       <c r="B9" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:3">
       <c r="B10" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:3">
       <c r="B11" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:3">
       <c r="B12" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:3">
       <c r="B13" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:3">
       <c r="B14" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:3">
       <c r="B15" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:3">
       <c r="B16" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.15">
+    <row r="17" spans="2:2">
       <c r="B17" s="1" t="s">
         <v>16</v>
       </c>

</xml_diff>

<commit_message>
anim fix and new masters
</commit_message>
<xml_diff>
--- a/pics.xlsx
+++ b/pics.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="28">
   <si>
     <t>01</t>
   </si>
@@ -102,6 +102,12 @@
   </si>
   <si>
     <t>600-699</t>
+  </si>
+  <si>
+    <t>700-799</t>
+  </si>
+  <si>
+    <t>800-899</t>
   </si>
 </sst>
 </file>
@@ -446,7 +452,7 @@
   <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+      <selection activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -510,35 +516,47 @@
       </c>
     </row>
     <row r="6" spans="1:3">
-      <c r="A6" t="s">
+      <c r="A6" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="2" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:3">
-      <c r="A7" t="s">
+      <c r="A7" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="2" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:3">
-      <c r="B8" s="1" t="s">
+      <c r="A8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" t="s">
         <v>7</v>
       </c>
+      <c r="C8" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="9" spans="1:3">
-      <c r="B9" s="1" t="s">
+      <c r="A9" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" t="s">
         <v>8</v>
+      </c>
+      <c r="C9" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:3">

</xml_diff>